<commit_message>
updated 00-OD-Prep to reflect the ZT208 resolution (in addition to values in the original ZT1259)
</commit_message>
<xml_diff>
--- a/data-raw/ZonificacionZT1259 complete.xlsx
+++ b/data-raw/ZonificacionZT1259 complete.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcmasteru365-my.sharepoint.com/personal/soukhoa_mcmaster_ca/Documents/05. PhD Research/05_Madrid-ZBE-LEZ/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="279" documentId="8_{F0E3EA1B-72AF-44CD-85F6-7BA03C107FCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EC7A00A-2040-4E4D-9A02-10662DD9AD76}"/>
+  <xr:revisionPtr revIDLastSave="285" documentId="8_{F0E3EA1B-72AF-44CD-85F6-7BA03C107FCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{94E197C9-DB3C-4BF6-A0A5-1C7455374D7D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1344" windowWidth="17280" windowHeight="10044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ZonificacionZT1259" sheetId="1" r:id="rId1"/>
@@ -5220,7 +5220,7 @@
   <dimension ref="A1:G1260"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="A1:H1"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>